<commit_message>
July 01 task updated with Array of employees
</commit_message>
<xml_diff>
--- a/01 July/Exceldata.xlsx
+++ b/01 July/Exceldata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
@@ -34,13 +34,22 @@
     <t>Age</t>
   </si>
   <si>
-    <t>kavin</t>
-  </si>
-  <si>
-    <t>8344442124</t>
-  </si>
-  <si>
-    <t>kavinkumar.prof@gmail.com</t>
+    <t>KAVIN</t>
+  </si>
+  <si>
+    <t>90876546</t>
+  </si>
+  <si>
+    <t>JKSDF</t>
+  </si>
+  <si>
+    <t>PRAVIN</t>
+  </si>
+  <si>
+    <t>089765467</t>
+  </si>
+  <si>
+    <t>SDFKJ</t>
   </si>
 </sst>
 </file>
@@ -381,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,7 +418,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -425,6 +434,26 @@
       </c>
       <c r="F2">
         <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>36489</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>